<commit_message>
Primera version para revision de indra con algunas correcciones, ejemplos y herramienta para comentarios
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-CodigoPaises.xlsx
+++ b/docs/StructureDefinition-CodigoPaises.xlsx
@@ -39,7 +39,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>PaisOrigenNacionalidadClLE</t>
+    <t>PaisOrigenClLE</t>
   </si>
   <si>
     <t>Title</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-01-25T13:45:37-03:00</t>
+    <t>2023-01-30T23:51:40-03:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>